<commit_message>
Se quitaron espacios del genero
</commit_message>
<xml_diff>
--- a/dataset_empleados.xlsx
+++ b/dataset_empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DireC\OneDrive\Documentos\IntegradorEstadisticaSecuela\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF16FA47-3DF8-4BFD-B0E5-4A3B4566E475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880C6954-7794-4192-907D-5F5D08244C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4EAD76-1B2F-4339-B8EB-A46405EF7F5F}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="106">
   <si>
     <t xml:space="preserve"> Licenciatura    </t>
   </si>
@@ -65,9 +65,6 @@
     <t xml:space="preserve"> Nueva York, EE. UU. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Masculino  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aplicación Móvil     </t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t xml:space="preserve"> San Francisco, EE. UU. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Femenino   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Análisis de Datos    </t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t xml:space="preserve"> Washington, D.C., EE. UU. </t>
   </si>
   <si>
-    <t xml:space="preserve"> No Binario </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ciberseguridad       </t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t xml:space="preserve"> Sídney, Australia </t>
   </si>
   <si>
-    <t xml:space="preserve"> Femenino </t>
-  </si>
-  <si>
     <t xml:space="preserve"> E-commerce </t>
   </si>
   <si>
@@ -170,9 +158,6 @@
     <t xml:space="preserve"> São Paulo, Brasil </t>
   </si>
   <si>
-    <t xml:space="preserve"> Masculino </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aplicaciones Móviles </t>
   </si>
   <si>
@@ -272,9 +257,6 @@
     <t>Agencia</t>
   </si>
   <si>
-    <t xml:space="preserve"> Femenino  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> JavaScript, Python    </t>
   </si>
   <si>
@@ -375,6 +357,15 @@
   </si>
   <si>
     <t>Ubicacion_Geografica</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>No Binario</t>
   </si>
 </sst>
 </file>
@@ -807,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE984B-E0EF-4115-AFA5-A2E460609B1A}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,40 +820,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I1" t="s">
-        <v>108</v>
-      </c>
       <c r="J1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -870,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -900,7 +891,7 @@
         <v>40</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -908,10 +899,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>35</v>
@@ -920,16 +911,16 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
       </c>
       <c r="J3">
         <v>80000</v>
@@ -938,7 +929,7 @@
         <v>45</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -946,7 +937,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -958,16 +949,16 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J4">
         <v>55000</v>
@@ -976,7 +967,7 @@
         <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -984,10 +975,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -996,16 +987,16 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>95000</v>
@@ -1014,7 +1005,7 @@
         <v>50</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1022,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1034,16 +1025,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" t="s">
         <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
       </c>
       <c r="J6">
         <v>62000</v>
@@ -1052,7 +1043,7 @@
         <v>38</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1060,10 +1051,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>32</v>
@@ -1075,13 +1066,13 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7">
         <v>72000</v>
@@ -1090,7 +1081,7 @@
         <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1098,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -1110,16 +1101,16 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>58000</v>
@@ -1128,7 +1119,7 @@
         <v>38</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1136,10 +1127,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>36</v>
@@ -1148,16 +1139,16 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J9">
         <v>85000</v>
@@ -1166,7 +1157,7 @@
         <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1174,7 +1165,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1186,16 +1177,16 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J10">
         <v>61000</v>
@@ -1204,7 +1195,7 @@
         <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1212,10 +1203,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>42</v>
@@ -1224,16 +1215,16 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J11">
         <v>92000</v>
@@ -1242,7 +1233,7 @@
         <v>45</v>
       </c>
       <c r="L11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1250,7 +1241,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -1262,16 +1253,16 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12">
         <v>64000</v>
@@ -1280,7 +1271,7 @@
         <v>42</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1288,10 +1279,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>37</v>
@@ -1300,10 +1291,10 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H13" t="s">
         <v>3</v>
@@ -1318,7 +1309,7 @@
         <v>47</v>
       </c>
       <c r="L13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1326,10 +1317,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>27</v>
@@ -1338,16 +1329,16 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J14">
         <v>54000</v>
@@ -1356,7 +1347,7 @@
         <v>41</v>
       </c>
       <c r="L14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1364,10 +1355,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>41</v>
@@ -1376,16 +1367,16 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
         <v>19</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
       </c>
       <c r="J15">
         <v>97000</v>
@@ -1394,7 +1385,7 @@
         <v>51</v>
       </c>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1402,10 +1393,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D16">
         <v>31</v>
@@ -1414,16 +1405,16 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" t="s">
         <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
       </c>
       <c r="J16">
         <v>63000</v>
@@ -1432,7 +1423,7 @@
         <v>40</v>
       </c>
       <c r="L16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1440,10 +1431,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>33</v>
@@ -1452,16 +1443,16 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J17">
         <v>71000</v>
@@ -1470,7 +1461,7 @@
         <v>46</v>
       </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1478,10 +1469,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D18">
         <v>29</v>
@@ -1490,16 +1481,16 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J18">
         <v>59000</v>
@@ -1508,7 +1499,7 @@
         <v>39</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1516,10 +1507,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>38</v>
@@ -1528,16 +1519,16 @@
         <v>13</v>
       </c>
       <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" t="s">
         <v>14</v>
-      </c>
-      <c r="G19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" t="s">
-        <v>16</v>
       </c>
       <c r="J19">
         <v>91000</v>
@@ -1546,7 +1537,7 @@
         <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1554,10 +1545,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D20">
         <v>32</v>
@@ -1566,16 +1557,16 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J20">
         <v>66000</v>
@@ -1584,7 +1575,7 @@
         <v>43</v>
       </c>
       <c r="L20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1592,10 +1583,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>35</v>
@@ -1604,16 +1595,16 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H21" t="s">
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J21">
         <v>82000</v>
@@ -1622,7 +1613,7 @@
         <v>49</v>
       </c>
       <c r="L21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1630,10 +1621,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D22">
         <v>28</v>
@@ -1642,13 +1633,13 @@
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
         <v>4</v>
@@ -1660,7 +1651,7 @@
         <v>41</v>
       </c>
       <c r="L22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1668,10 +1659,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D23">
         <v>36</v>
@@ -1680,16 +1671,16 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J23">
         <v>71000</v>
@@ -1698,7 +1689,7 @@
         <v>47</v>
       </c>
       <c r="L23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1706,10 +1697,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D24">
         <v>30</v>
@@ -1718,16 +1709,16 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" t="s">
         <v>14</v>
-      </c>
-      <c r="G24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" t="s">
-        <v>16</v>
       </c>
       <c r="J24">
         <v>64000</v>
@@ -1736,7 +1727,7 @@
         <v>39</v>
       </c>
       <c r="L24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1744,10 +1735,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D25">
         <v>42</v>
@@ -1756,16 +1747,16 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" t="s">
         <v>19</v>
-      </c>
-      <c r="G25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>21</v>
       </c>
       <c r="J25">
         <v>93000</v>
@@ -1774,7 +1765,7 @@
         <v>50</v>
       </c>
       <c r="L25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1782,10 +1773,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <v>31</v>
@@ -1794,16 +1785,16 @@
         <v>6</v>
       </c>
       <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" t="s">
         <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" t="s">
-        <v>25</v>
       </c>
       <c r="J26">
         <v>61000</v>
@@ -1812,7 +1803,7 @@
         <v>39</v>
       </c>
       <c r="L26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1820,10 +1811,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>34</v>
@@ -1832,16 +1823,16 @@
         <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J27">
         <v>84000</v>
@@ -1850,7 +1841,7 @@
         <v>45</v>
       </c>
       <c r="L27" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1858,10 +1849,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D28">
         <v>29</v>
@@ -1870,16 +1861,16 @@
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J28">
         <v>57000</v>
@@ -1888,7 +1879,7 @@
         <v>38</v>
       </c>
       <c r="L28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1896,10 +1887,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D29">
         <v>41</v>
@@ -1908,13 +1899,13 @@
         <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I29" t="s">
         <v>4</v>
@@ -1926,7 +1917,7 @@
         <v>49</v>
       </c>
       <c r="L29" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1934,10 +1925,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D30">
         <v>32</v>
@@ -1946,16 +1937,16 @@
         <v>8</v>
       </c>
       <c r="F30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" t="s">
         <v>23</v>
-      </c>
-      <c r="G30" t="s">
-        <v>71</v>
-      </c>
-      <c r="H30" t="s">
-        <v>73</v>
-      </c>
-      <c r="I30" t="s">
-        <v>25</v>
       </c>
       <c r="J30">
         <v>62000</v>
@@ -1964,7 +1955,7 @@
         <v>41</v>
       </c>
       <c r="L30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1972,10 +1963,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D31">
         <v>33</v>
@@ -1984,16 +1975,16 @@
         <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G31" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J31">
         <v>72000</v>
@@ -2002,7 +1993,7 @@
         <v>46</v>
       </c>
       <c r="L31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2010,10 +2001,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32">
         <v>39</v>
@@ -2022,16 +2013,16 @@
         <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H32" t="s">
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J32">
         <v>82000</v>
@@ -2040,7 +2031,7 @@
         <v>42</v>
       </c>
       <c r="L32" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2048,7 +2039,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -2060,16 +2051,16 @@
         <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I33" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J33">
         <v>76000</v>
@@ -2078,7 +2069,7 @@
         <v>44</v>
       </c>
       <c r="L33" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2086,10 +2077,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D34">
         <v>35</v>
@@ -2098,16 +2089,16 @@
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H34" t="s">
         <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J34">
         <v>69000</v>
@@ -2116,7 +2107,7 @@
         <v>38</v>
       </c>
       <c r="L34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2124,10 +2115,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D35">
         <v>42</v>
@@ -2136,16 +2127,16 @@
         <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J35">
         <v>95000</v>
@@ -2154,7 +2145,7 @@
         <v>47</v>
       </c>
       <c r="L35" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2162,10 +2153,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>34</v>
@@ -2174,16 +2165,16 @@
         <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H36" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J36">
         <v>78000</v>
@@ -2192,7 +2183,7 @@
         <v>43</v>
       </c>
       <c r="L36" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2200,7 +2191,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
@@ -2212,16 +2203,16 @@
         <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G37" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H37" t="s">
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J37">
         <v>69000</v>
@@ -2230,7 +2221,7 @@
         <v>40</v>
       </c>
       <c r="L37" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2238,10 +2229,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38">
         <v>36</v>
@@ -2250,16 +2241,16 @@
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H38" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J38">
         <v>78000</v>
@@ -2268,7 +2259,7 @@
         <v>45</v>
       </c>
       <c r="L38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2276,10 +2267,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D39">
         <v>32</v>
@@ -2288,16 +2279,16 @@
         <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H39" t="s">
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J39">
         <v>72000</v>
@@ -2306,7 +2297,7 @@
         <v>42</v>
       </c>
       <c r="L39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2314,10 +2305,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D40">
         <v>41</v>
@@ -2326,16 +2317,16 @@
         <v>14</v>
       </c>
       <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" t="s">
+        <v>84</v>
+      </c>
+      <c r="I40" t="s">
         <v>19</v>
-      </c>
-      <c r="G40" t="s">
-        <v>54</v>
-      </c>
-      <c r="H40" t="s">
-        <v>90</v>
-      </c>
-      <c r="I40" t="s">
-        <v>21</v>
       </c>
       <c r="J40">
         <v>91000</v>
@@ -2344,7 +2335,7 @@
         <v>50</v>
       </c>
       <c r="L40" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2352,10 +2343,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41">
         <v>33</v>
@@ -2364,16 +2355,16 @@
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G41" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H41" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I41" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J41">
         <v>73000</v>
@@ -2382,7 +2373,7 @@
         <v>41</v>
       </c>
       <c r="L41" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2390,7 +2381,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -2402,13 +2393,13 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H42" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I42" t="s">
         <v>4</v>
@@ -2420,7 +2411,7 @@
         <v>40</v>
       </c>
       <c r="L42" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2428,10 +2419,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43">
         <v>40</v>
@@ -2440,16 +2431,16 @@
         <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G43" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J43">
         <v>89000</v>
@@ -2458,7 +2449,7 @@
         <v>45</v>
       </c>
       <c r="L43" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2466,10 +2457,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44">
         <v>37</v>
@@ -2478,16 +2469,16 @@
         <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G44" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H44" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" t="s">
         <v>10</v>
-      </c>
-      <c r="I44" t="s">
-        <v>11</v>
       </c>
       <c r="J44">
         <v>81000</v>
@@ -2496,7 +2487,7 @@
         <v>47</v>
       </c>
       <c r="L44" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2504,7 +2495,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
@@ -2516,16 +2507,16 @@
         <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G45" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H45" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I45" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J45">
         <v>72000</v>
@@ -2534,7 +2525,7 @@
         <v>42</v>
       </c>
       <c r="L45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2542,10 +2533,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D46">
         <v>42</v>
@@ -2554,16 +2545,16 @@
         <v>14</v>
       </c>
       <c r="F46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" t="s">
         <v>19</v>
-      </c>
-      <c r="G46" t="s">
-        <v>54</v>
-      </c>
-      <c r="H46" t="s">
-        <v>10</v>
-      </c>
-      <c r="I46" t="s">
-        <v>21</v>
       </c>
       <c r="J46">
         <v>93000</v>
@@ -2572,7 +2563,7 @@
         <v>48</v>
       </c>
       <c r="L46" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2580,10 +2571,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47">
         <v>34</v>
@@ -2592,16 +2583,16 @@
         <v>9</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H47" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I47" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J47">
         <v>75000</v>
@@ -2610,7 +2601,7 @@
         <v>43</v>
       </c>
       <c r="L47" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2618,7 +2609,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
@@ -2630,13 +2621,13 @@
         <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G48" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H48" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I48" t="s">
         <v>4</v>
@@ -2648,7 +2639,7 @@
         <v>41</v>
       </c>
       <c r="L48" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2656,10 +2647,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49">
         <v>36</v>
@@ -2668,16 +2659,16 @@
         <v>11</v>
       </c>
       <c r="F49" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G49" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I49" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J49">
         <v>82000</v>
@@ -2686,7 +2677,7 @@
         <v>47</v>
       </c>
       <c r="L49" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2694,10 +2685,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D50">
         <v>32</v>
@@ -2706,16 +2697,16 @@
         <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G50" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H50" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I50" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J50">
         <v>70000</v>
@@ -2724,7 +2715,7 @@
         <v>45</v>
       </c>
       <c r="L50" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>